<commit_message>
Task 7. Created advanced pivot table with Timeline, Slicer and field Profit = 30%
</commit_message>
<xml_diff>
--- a/day2/Task 5/dax_model.xlsx
+++ b/day2/Task 5/dax_model.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Andrii\Documents\Data Analyst - Andrew Bootcamp\da-bootcamp-2025\da-bootcamp-2025\day2\Task 5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2973A84E-01A5-46A1-B9B0-491157928642}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03F1FFF4-362C-4D16-98A7-CD12C519E3FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
   </definedNames>
   <calcPr calcId="0"/>
   <pivotCaches>
-    <pivotCache cacheId="16" r:id="rId3"/>
+    <pivotCache cacheId="28" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{FCE2AD5D-F65C-4FA6-A056-5C36A1767C68}">
@@ -192,7 +192,31 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="18">
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="13" formatCode="0%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="13" formatCode="0%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="13" formatCode="0%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="13" formatCode="0%"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="13" formatCode="0%"/>
     </dxf>
@@ -271,7 +295,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" saveData="0" refreshedBy="Andrii" refreshedDate="46024.65696388889" backgroundQuery="1" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1" xr:uid="{5FFE165B-3DD4-48D8-92A2-D937665A7D42}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" saveData="0" refreshedBy="Andrii" refreshedDate="46024.658914120373" backgroundQuery="1" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1" xr:uid="{5FFE165B-3DD4-48D8-92A2-D937665A7D42}">
   <cacheSource type="external" connectionId="1"/>
   <cacheFields count="3">
     <cacheField name="[Measures].[AvgPrice]" caption="AvgPrice" numFmtId="0" hierarchy="4" level="32767"/>
@@ -336,12 +360,12 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{826CA619-1C9C-4C28-B70A-C3569B29375C}" name="PivotTable2" cacheId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{826CA619-1C9C-4C28-B70A-C3569B29375C}" name="PivotTable2" cacheId="28" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:C16" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField dataField="1" subtotalTop="0" showAll="0" defaultSubtotal="0"/>
     <pivotField dataField="1" subtotalTop="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField axis="axisRow" allDrilled="1" subtotalTop="0" showAll="0" dataSourceSort="1" defaultSubtotal="0" defaultAttributeDrillState="1">
+    <pivotField axis="axisRow" allDrilled="1" subtotalTop="0" showAll="0" sortType="descending" defaultSubtotal="0" defaultAttributeDrillState="1">
       <items count="12">
         <item x="0"/>
         <item x="1"/>
@@ -356,6 +380,15 @@
         <item x="10"/>
         <item x="11"/>
       </items>
+      <autoSortScope>
+        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
+          <references count="1">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </autoSortScope>
     </pivotField>
   </pivotFields>
   <rowFields count="1">
@@ -363,22 +396,19 @@
   </rowFields>
   <rowItems count="13">
     <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
       <x/>
     </i>
     <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
+      <x v="9"/>
     </i>
     <i>
       <x v="6"/>
@@ -387,16 +417,19 @@
       <x v="7"/>
     </i>
     <i>
-      <x v="8"/>
+      <x v="4"/>
     </i>
     <i>
-      <x v="9"/>
+      <x v="1"/>
     </i>
     <i>
-      <x v="10"/>
+      <x v="3"/>
     </i>
     <i>
       <x v="11"/>
+    </i>
+    <i>
+      <x v="8"/>
     </i>
     <i t="grand">
       <x/>
@@ -418,14 +451,14 @@
     <dataField fld="1" subtotal="count" baseField="0" baseItem="0" numFmtId="9"/>
   </dataFields>
   <formats count="2">
-    <format dxfId="3">
+    <format dxfId="11">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="2" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="0">
+    <format dxfId="8">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
@@ -469,7 +502,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{38D3650D-34D2-4D63-9C2C-B6C9173FCF65}" name="RawTable" displayName="RawTable" ref="A1:D3046" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="8" tableBorderDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{38D3650D-34D2-4D63-9C2C-B6C9173FCF65}" name="RawTable" displayName="RawTable" ref="A1:D3046" totalsRowShown="0" headerRowDxfId="15" headerRowBorderDxfId="16" tableBorderDxfId="17">
   <autoFilter ref="A1:D3046" xr:uid="{38D3650D-34D2-4D63-9C2C-B6C9173FCF65}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{EE8C0944-D593-4F79-AA8E-08E71734A646}" name="District"/>
@@ -769,13 +802,14 @@
   <dimension ref="A3:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -791,134 +825,134 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B4" s="5">
-        <v>3649.212598425197</v>
+        <v>3849.6062992125985</v>
       </c>
       <c r="C4" s="6">
-        <v>8.5806197782869312E-2</v>
+        <v>9.0518179083061395E-2</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B5" s="5">
-        <v>3446.6403162055335</v>
+        <v>3847.0355731225295</v>
       </c>
       <c r="C5" s="6">
-        <v>8.0723923256728919E-2</v>
+        <v>9.0101599203869565E-2</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B6" s="5">
-        <v>3849.6062992125985</v>
+        <v>3846.6535433070867</v>
       </c>
       <c r="C6" s="6">
-        <v>9.0518179083061395E-2</v>
+        <v>9.0448749103196099E-2</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B7" s="5">
-        <v>3249.803149606299</v>
+        <v>3649.212598425197</v>
       </c>
       <c r="C7" s="6">
-        <v>7.6414635839755607E-2</v>
+        <v>8.5806197782869312E-2</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B8" s="5">
-        <v>3447.2440944881891</v>
+        <v>3647.6377952755906</v>
       </c>
       <c r="C8" s="6">
-        <v>8.1057187160082395E-2</v>
+        <v>8.5769168460274478E-2</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B9" s="5">
-        <v>3846.6535433070867</v>
+        <v>3646.8379446640315</v>
       </c>
       <c r="C9" s="6">
-        <v>9.0448749103196099E-2</v>
+        <v>8.5412761230299242E-2</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="B10" s="5">
-        <v>3646.8379446640315</v>
+        <v>3450.196850393701</v>
       </c>
       <c r="C10" s="6">
-        <v>8.5412761230299242E-2</v>
+        <v>8.112661713994769E-2</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B11" s="5">
-        <v>3450.196850393701</v>
+        <v>3447.2440944881891</v>
       </c>
       <c r="C11" s="6">
-        <v>8.112661713994769E-2</v>
+        <v>8.1057187160082395E-2</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B12" s="5">
-        <v>3243.8976377952754</v>
+        <v>3446.6403162055335</v>
       </c>
       <c r="C12" s="6">
-        <v>7.6275775880025001E-2</v>
+        <v>8.0723923256728919E-2</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B13" s="5">
-        <v>3647.6377952755906</v>
+        <v>3249.803149606299</v>
       </c>
       <c r="C13" s="6">
-        <v>8.5769168460274478E-2</v>
+        <v>7.6414635839755607E-2</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B14" s="5">
-        <v>3847.0355731225295</v>
+        <v>3246.8503937007872</v>
       </c>
       <c r="C14" s="6">
-        <v>9.0101599203869565E-2</v>
+        <v>7.6345205859890297E-2</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B15" s="5">
-        <v>3246.8503937007872</v>
+        <v>3243.8976377952754</v>
       </c>
       <c r="C15" s="6">
-        <v>7.6345205859890297E-2</v>
+        <v>7.6275775880025001E-2</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>